<commit_message>
create new branch for SaaS and edit the pwd locator at login page
</commit_message>
<xml_diff>
--- a/Data/DataTest.xlsx
+++ b/Data/DataTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JavaProject\Parallel\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72EEFF2-75E0-4132-BB23-4DA8D909654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DCB59D-67FC-47AF-97AA-66CC8094CF55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -68,9 +68,6 @@
     <t>SecureDoc Enterprise for Linux</t>
   </si>
   <si>
-    <t>SecureDoc for OSA</t>
-  </si>
-  <si>
     <t>Windows-Endpoint</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>Linux-Endpoint</t>
-  </si>
-  <si>
-    <t>OSA-Endpoint</t>
   </si>
   <si>
     <t>hello work</t>
@@ -468,10 +462,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F23598-F70D-408D-AEED-D1DE84F85863}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -498,10 +492,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -512,10 +506,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -526,30 +520,16 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -559,10 +539,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17275F52-E661-4D4E-ACD5-E18F8564A9B9}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E5"/>
+      <selection activeCell="A5" sqref="A5:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -578,16 +558,16 @@
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -598,13 +578,13 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -615,13 +595,13 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -632,30 +612,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>